<commit_message>
replacing a static excel file with one that has dynamic cell references
</commit_message>
<xml_diff>
--- a/spreadsheets/manager_preferences.xlsx
+++ b/spreadsheets/manager_preferences.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1ac4eaab54ff55ac/Desktop/REPOS/job_scheduling/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="130" documentId="11_68D9B4D9EA67C8701C0992CE73840BD4244323B2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BDAF4BC-7BA7-4B9C-BE19-AE981972C28E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="days_off" sheetId="1" r:id="rId1"/>
@@ -25,7 +31,18 @@
     <sheet name="Rob" sheetId="16" r:id="rId16"/>
     <sheet name="Mads" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -128,8 +145,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,13 +209,25 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -236,7 +265,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -270,6 +299,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -304,9 +334,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -479,19 +510,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -499,7 +530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -513,14 +544,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -540,168 +573,210 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
+        <f>default_preferences!B2</f>
         <v>10</v>
       </c>
       <c r="C2">
+        <f>default_preferences!C2</f>
         <v>10</v>
       </c>
       <c r="D2">
+        <f>default_preferences!D2</f>
         <v>10</v>
       </c>
       <c r="E2">
+        <f>default_preferences!E2</f>
         <v>10</v>
       </c>
       <c r="F2">
+        <f>default_preferences!F2</f>
         <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8">
+        <f>default_preferences!B8</f>
         <v>10</v>
       </c>
       <c r="C8">
+        <f>default_preferences!C8</f>
         <v>10</v>
       </c>
       <c r="D8">
+        <f>default_preferences!D8</f>
         <v>10</v>
       </c>
       <c r="E8">
+        <f>default_preferences!E8</f>
         <v>10</v>
       </c>
       <c r="F8">
+        <f>default_preferences!F8</f>
         <v>10</v>
       </c>
       <c r="G8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <f>default_preferences!G8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -724,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -747,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -770,72 +845,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -845,14 +938,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -872,7 +967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -895,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -918,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -941,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -964,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -987,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1010,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1033,53 +1128,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9">
+        <f>default_preferences!B9</f>
         <v>10</v>
       </c>
       <c r="C9">
+        <f>default_preferences!C9</f>
         <v>10</v>
       </c>
       <c r="D9">
+        <f>default_preferences!D9</f>
         <v>10</v>
       </c>
       <c r="E9">
+        <f>default_preferences!E9</f>
         <v>10</v>
       </c>
       <c r="F9">
+        <f>default_preferences!F9</f>
         <v>10</v>
       </c>
       <c r="G9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <f>default_preferences!G9</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10">
+        <f>default_preferences!B10</f>
         <v>10</v>
       </c>
       <c r="C10">
+        <f>default_preferences!C10</f>
         <v>10</v>
       </c>
       <c r="D10">
+        <f>default_preferences!D10</f>
         <v>10</v>
       </c>
       <c r="E10">
+        <f>default_preferences!E10</f>
         <v>10</v>
       </c>
       <c r="F10">
+        <f>default_preferences!F10</f>
         <v>10</v>
       </c>
       <c r="G10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <f>default_preferences!G10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1102,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1125,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1148,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1177,14 +1284,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1227,191 +1336,239 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8">
+        <f>default_preferences!B8</f>
         <v>10</v>
       </c>
       <c r="C8">
+        <f>default_preferences!C8</f>
         <v>10</v>
       </c>
       <c r="D8">
+        <f>default_preferences!D8</f>
         <v>10</v>
       </c>
       <c r="E8">
+        <f>default_preferences!E8</f>
         <v>10</v>
       </c>
       <c r="F8">
+        <f>default_preferences!F8</f>
         <v>10</v>
       </c>
       <c r="G8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <f>default_preferences!G8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9">
+        <f>default_preferences!B9</f>
         <v>10</v>
       </c>
       <c r="C9">
+        <f>default_preferences!C9</f>
         <v>10</v>
       </c>
       <c r="D9">
+        <f>default_preferences!D9</f>
         <v>10</v>
       </c>
       <c r="E9">
+        <f>default_preferences!E9</f>
         <v>10</v>
       </c>
       <c r="F9">
+        <f>default_preferences!F9</f>
         <v>10</v>
       </c>
       <c r="G9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <f>default_preferences!G9</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10">
+        <f>default_preferences!B10</f>
         <v>10</v>
       </c>
       <c r="C10">
+        <f>default_preferences!C10</f>
         <v>10</v>
       </c>
       <c r="D10">
+        <f>default_preferences!D10</f>
         <v>10</v>
       </c>
       <c r="E10">
+        <f>default_preferences!E10</f>
         <v>10</v>
       </c>
       <c r="F10">
+        <f>default_preferences!F10</f>
         <v>10</v>
       </c>
       <c r="G10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <f>default_preferences!G10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1434,72 +1591,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -1509,14 +1684,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1559,30 +1736,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1605,7 +1788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1628,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1651,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1674,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1697,53 +1880,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <f>default_preferences!B9</f>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <f>default_preferences!C9</f>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <f>default_preferences!D9</f>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <f>default_preferences!E9</f>
+        <v>10</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <f>default_preferences!F9</f>
+        <v>10</v>
       </c>
       <c r="G9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <f>default_preferences!G9</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <f>default_preferences!B10</f>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <f>default_preferences!C10</f>
+        <v>10</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <f>default_preferences!D10</f>
+        <v>10</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <f>default_preferences!E10</f>
+        <v>10</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <f>default_preferences!F10</f>
+        <v>10</v>
       </c>
       <c r="G10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <f>default_preferences!G10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -1766,72 +1961,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -1841,14 +2054,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1868,145 +2083,181 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
+        <f>default_preferences!B2</f>
         <v>10</v>
       </c>
       <c r="C2">
+        <f>default_preferences!C2</f>
         <v>10</v>
       </c>
       <c r="D2">
+        <f>default_preferences!D2</f>
         <v>10</v>
       </c>
       <c r="E2">
+        <f>default_preferences!E2</f>
         <v>10</v>
       </c>
       <c r="F2">
+        <f>default_preferences!F2</f>
         <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2029,7 +2280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2052,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -2075,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -2098,72 +2349,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -2173,14 +2442,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2200,145 +2471,181 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>default_preferences!B2</f>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <f>default_preferences!C2</f>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>default_preferences!D2</f>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>default_preferences!E2</f>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <f>default_preferences!F2</f>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2361,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -2384,7 +2691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -2407,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -2430,72 +2737,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -2505,14 +2830,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2532,7 +2859,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2555,122 +2882,152 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -2693,53 +3050,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9">
+        <f>default_preferences!B9</f>
         <v>10</v>
       </c>
       <c r="C9">
+        <f>default_preferences!C9</f>
         <v>10</v>
       </c>
       <c r="D9">
+        <f>default_preferences!D9</f>
         <v>10</v>
       </c>
       <c r="E9">
+        <f>default_preferences!E9</f>
         <v>10</v>
       </c>
       <c r="F9">
+        <f>default_preferences!F9</f>
         <v>10</v>
       </c>
       <c r="G9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <f>default_preferences!G9</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10">
+        <f>default_preferences!B10</f>
         <v>10</v>
       </c>
       <c r="C10">
+        <f>default_preferences!C10</f>
         <v>10</v>
       </c>
       <c r="D10">
+        <f>default_preferences!D10</f>
         <v>10</v>
       </c>
       <c r="E10">
+        <f>default_preferences!E10</f>
         <v>10</v>
       </c>
       <c r="F10">
+        <f>default_preferences!F10</f>
         <v>10</v>
       </c>
       <c r="G10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <f>default_preferences!G10</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -2762,72 +3131,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -2837,14 +3224,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2864,145 +3253,181 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <f>default_preferences!B2</f>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <f>default_preferences!C2</f>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>default_preferences!D2</f>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <f>default_preferences!E2</f>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <f>default_preferences!F2</f>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -3025,7 +3450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -3048,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3071,7 +3496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3094,72 +3519,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -3169,14 +3612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3184,7 +3627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3198,14 +3641,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3213,7 +3656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3221,7 +3664,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3229,7 +3672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3243,14 +3686,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -3270,7 +3715,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -3293,7 +3738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -3316,7 +3761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -3339,7 +3784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -3362,7 +3807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -3385,7 +3830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -3408,7 +3853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -3431,7 +3876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -3454,7 +3899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3477,7 +3922,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3500,7 +3945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -3523,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -3546,7 +3991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -3575,14 +4020,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -3602,168 +4052,210 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
+        <f>default_preferences!B2</f>
         <v>10</v>
       </c>
       <c r="C2">
+        <f>default_preferences!C2</f>
         <v>10</v>
       </c>
       <c r="D2">
+        <f>default_preferences!D2</f>
         <v>10</v>
       </c>
       <c r="E2">
+        <f>default_preferences!E2</f>
         <v>10</v>
       </c>
       <c r="F2">
+        <f>default_preferences!F2</f>
         <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8">
+        <f>default_preferences!B8</f>
         <v>10</v>
       </c>
       <c r="C8">
+        <f>default_preferences!C8</f>
         <v>10</v>
       </c>
       <c r="D8">
+        <f>default_preferences!D8</f>
         <v>10</v>
       </c>
       <c r="E8">
+        <f>default_preferences!E8</f>
         <v>10</v>
       </c>
       <c r="F8">
+        <f>default_preferences!F8</f>
         <v>10</v>
       </c>
       <c r="G8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <f>default_preferences!G8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -3786,7 +4278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -3809,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -3832,72 +4324,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -3907,14 +4417,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -3934,7 +4449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -3957,145 +4472,181 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B8">
+        <f>default_preferences!B8</f>
         <v>10</v>
       </c>
       <c r="C8">
+        <f>default_preferences!C8</f>
         <v>10</v>
       </c>
       <c r="D8">
+        <f>default_preferences!D8</f>
         <v>10</v>
       </c>
       <c r="E8">
+        <f>default_preferences!E8</f>
         <v>10</v>
       </c>
       <c r="F8">
+        <f>default_preferences!F8</f>
         <v>10</v>
       </c>
       <c r="G8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <f>default_preferences!G8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -4118,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -4141,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -4164,72 +4715,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -4239,14 +4808,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -4266,145 +4837,181 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
+        <f>default_preferences!B2</f>
         <v>10</v>
       </c>
       <c r="C2">
+        <f>default_preferences!C2</f>
         <v>10</v>
       </c>
       <c r="D2">
+        <f>default_preferences!D2</f>
         <v>10</v>
       </c>
       <c r="E2">
+        <f>default_preferences!E2</f>
         <v>10</v>
       </c>
       <c r="F2">
+        <f>default_preferences!F2</f>
         <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -4427,7 +5034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -4450,7 +5057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -4473,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -4496,72 +5103,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -4571,14 +5196,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -4598,145 +5225,181 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
+        <f>default_preferences!B2</f>
         <v>10</v>
       </c>
       <c r="C2">
+        <f>default_preferences!C2</f>
         <v>10</v>
       </c>
       <c r="D2">
+        <f>default_preferences!D2</f>
         <v>10</v>
       </c>
       <c r="E2">
+        <f>default_preferences!E2</f>
         <v>10</v>
       </c>
       <c r="F2">
+        <f>default_preferences!F2</f>
         <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -4759,7 +5422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -4782,7 +5445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -4805,95 +5468,119 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B11">
+        <f>default_preferences!B11</f>
         <v>10</v>
       </c>
       <c r="C11">
+        <f>default_preferences!C11</f>
         <v>10</v>
       </c>
       <c r="D11">
+        <f>default_preferences!D11</f>
         <v>10</v>
       </c>
       <c r="E11">
+        <f>default_preferences!E11</f>
         <v>10</v>
       </c>
       <c r="F11">
+        <f>default_preferences!F11</f>
         <v>10</v>
       </c>
       <c r="G11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <f>default_preferences!G11</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>
@@ -4903,14 +5590,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -4930,145 +5619,181 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B2">
+        <f>default_preferences!B2</f>
         <v>10</v>
       </c>
       <c r="C2">
+        <f>default_preferences!C2</f>
         <v>10</v>
       </c>
       <c r="D2">
+        <f>default_preferences!D2</f>
         <v>10</v>
       </c>
       <c r="E2">
+        <f>default_preferences!E2</f>
         <v>10</v>
       </c>
       <c r="F2">
+        <f>default_preferences!F2</f>
         <v>10</v>
       </c>
       <c r="G2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f>default_preferences!G2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <f>default_preferences!B3</f>
         <v>4</v>
       </c>
       <c r="C3">
+        <f>default_preferences!C3</f>
         <v>4</v>
       </c>
       <c r="D3">
+        <f>default_preferences!D3</f>
         <v>4</v>
       </c>
       <c r="E3">
+        <f>default_preferences!E3</f>
         <v>4</v>
       </c>
       <c r="F3">
+        <f>default_preferences!F3</f>
         <v>4</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <f>default_preferences!G3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4">
+        <f>default_preferences!B4</f>
         <v>10</v>
       </c>
       <c r="C4">
+        <f>default_preferences!C4</f>
         <v>10</v>
       </c>
       <c r="D4">
+        <f>default_preferences!D4</f>
         <v>10</v>
       </c>
       <c r="E4">
+        <f>default_preferences!E4</f>
         <v>10</v>
       </c>
       <c r="F4">
+        <f>default_preferences!F4</f>
         <v>10</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f>default_preferences!G4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5">
+        <f>default_preferences!B5</f>
         <v>10</v>
       </c>
       <c r="C5">
+        <f>default_preferences!C5</f>
         <v>10</v>
       </c>
       <c r="D5">
+        <f>default_preferences!D5</f>
         <v>10</v>
       </c>
       <c r="E5">
+        <f>default_preferences!E5</f>
         <v>10</v>
       </c>
       <c r="F5">
+        <f>default_preferences!F5</f>
         <v>10</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <f>default_preferences!G5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B6">
+        <f>default_preferences!B6</f>
         <v>10</v>
       </c>
       <c r="C6">
+        <f>default_preferences!C6</f>
         <v>5</v>
       </c>
       <c r="D6">
+        <f>default_preferences!D6</f>
         <v>5</v>
       </c>
       <c r="E6">
+        <f>default_preferences!E6</f>
         <v>5</v>
       </c>
       <c r="F6">
+        <f>default_preferences!F6</f>
         <v>5</v>
       </c>
       <c r="G6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <f>default_preferences!G6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7">
+        <f>default_preferences!B7</f>
         <v>3</v>
       </c>
       <c r="C7">
+        <f>default_preferences!C7</f>
         <v>1</v>
       </c>
       <c r="D7">
+        <f>default_preferences!D7</f>
         <v>1</v>
       </c>
       <c r="E7">
+        <f>default_preferences!E7</f>
         <v>1</v>
       </c>
       <c r="F7">
+        <f>default_preferences!F7</f>
         <v>1</v>
       </c>
       <c r="G7">
+        <f>default_preferences!G7</f>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -5091,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -5114,7 +5839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -5137,7 +5862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -5160,72 +5885,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B12">
+        <f>default_preferences!B12</f>
         <v>1</v>
       </c>
       <c r="C12">
+        <f>default_preferences!C12</f>
         <v>4</v>
       </c>
       <c r="D12">
+        <f>default_preferences!D12</f>
         <v>2.5</v>
       </c>
       <c r="E12">
+        <f>default_preferences!E12</f>
         <v>1</v>
       </c>
       <c r="F12">
+        <f>default_preferences!F12</f>
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <f>default_preferences!G12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13">
+        <f>default_preferences!B13</f>
         <v>1</v>
       </c>
       <c r="C13">
+        <f>default_preferences!C13</f>
         <v>4</v>
       </c>
       <c r="D13">
+        <f>default_preferences!D13</f>
         <v>2.5</v>
       </c>
       <c r="E13">
+        <f>default_preferences!E13</f>
         <v>1</v>
       </c>
       <c r="F13">
+        <f>default_preferences!F13</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <f>default_preferences!G13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B14">
+        <f>default_preferences!B14</f>
         <v>1</v>
       </c>
       <c r="C14">
+        <f>default_preferences!C14</f>
         <v>4</v>
       </c>
       <c r="D14">
+        <f>default_preferences!D14</f>
         <v>2.5</v>
       </c>
       <c r="E14">
+        <f>default_preferences!E14</f>
         <v>1</v>
       </c>
       <c r="F14">
+        <f>default_preferences!F14</f>
         <v>0</v>
       </c>
       <c r="G14">
+        <f>default_preferences!G14</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>